<commit_message>
updates on processing FIN001-report-checkpoint. Missing pychk date
</commit_message>
<xml_diff>
--- a/test/RFL Master File_7.17.25_small_sample_2.xlsx
+++ b/test/RFL Master File_7.17.25_small_sample_2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awidjaja\Documents\RFL- POC\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57936B0A-4E86-47DF-B629-4DC828AC77DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311A331E-41B3-42AF-8016-091F25B8F8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33255" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{C0D895A2-B84E-46DB-A012-849BB42E6BC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C0D895A2-B84E-46DB-A012-849BB42E6BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="exception" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="48">
   <si>
     <t>Business Unit</t>
   </si>
@@ -168,6 +169,18 @@
   </si>
   <si>
     <t>Corbin,Camilla</t>
+  </si>
+  <si>
+    <t>Actual Payroll Status in Job Data</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Payroll Status is not Active</t>
+  </si>
+  <si>
+    <t>Arrears detected</t>
   </si>
 </sst>
 </file>
@@ -212,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -235,11 +248,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -247,6 +271,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C784EE-8980-4C62-87F3-2DA06815614F}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,9 +625,10 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,8 +668,11 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -681,8 +712,11 @@
       <c r="M2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -722,8 +756,11 @@
       <c r="M3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -763,8 +800,11 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -804,8 +844,11 @@
       <c r="M5" s="3">
         <v>1023635945846</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -846,7 +889,7 @@
         <v>1040293045846</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -887,7 +930,7 @@
         <v>1060634045846</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -928,7 +971,7 @@
         <v>1078677245846</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -969,7 +1012,7 @@
         <v>1010522145846</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1010,7 +1053,7 @@
         <v>1010883545845</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1049,6 +1092,166 @@
       </c>
       <c r="M11" s="3">
         <v>1010949645845</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215BA176-A211-4AF1-BCC6-E15647AA23F6}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="37.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>10195831</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45846</v>
+      </c>
+      <c r="H2" s="2">
+        <v>45763</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10236359</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4">
+        <v>45846</v>
+      </c>
+      <c r="H3" s="4">
+        <v>45831</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1023635945846</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update as of 10/23/2024
</commit_message>
<xml_diff>
--- a/test/RFL Master File_7.17.25_small_sample_2.xlsx
+++ b/test/RFL Master File_7.17.25_small_sample_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awidjaja\Documents\RFL- POC\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311A331E-41B3-42AF-8016-091F25B8F8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4EED2B-DD33-430A-A705-B39BB0938151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C0D895A2-B84E-46DB-A012-849BB42E6BC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0D895A2-B84E-46DB-A012-849BB42E6BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="60">
   <si>
     <t>Business Unit</t>
   </si>
@@ -181,13 +181,49 @@
   </si>
   <si>
     <t>Arrears detected</t>
+  </si>
+  <si>
+    <t>SDCMP</t>
+  </si>
+  <si>
+    <t>Shan,Tianyi</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Short Work Break</t>
+  </si>
+  <si>
+    <t>6AC</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>1036555745931</t>
+  </si>
+  <si>
+    <t>IRCMP</t>
+  </si>
+  <si>
+    <t>Cho,Julie Grace</t>
+  </si>
+  <si>
+    <t>9AC</t>
+  </si>
+  <si>
+    <t>1029075745931</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +242,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -274,6 +326,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C784EE-8980-4C62-87F3-2DA06815614F}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,13 +680,12 @@
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,10 +704,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -668,11 +725,8 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -712,11 +766,8 @@
       <c r="M2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -756,11 +807,8 @@
       <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="N3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -800,15 +848,12 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="9">
         <v>10236359</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -844,11 +889,8 @@
       <c r="M5" s="3">
         <v>1023635945846</v>
       </c>
-      <c r="N5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -889,7 +931,7 @@
         <v>1040293045846</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -930,7 +972,7 @@
         <v>1060634045846</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -971,7 +1013,7 @@
         <v>1078677245846</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1012,7 +1054,7 @@
         <v>1010522145846</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1053,7 +1095,7 @@
         <v>1010883545845</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1092,6 +1134,103 @@
       </c>
       <c r="M11" s="3">
         <v>1010949645845</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="7">
+        <v>10365557</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="8">
+        <v>45931</v>
+      </c>
+      <c r="H12" s="8">
+        <v>45911</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="7">
+        <v>3</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10290757</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="8">
+        <v>45931</v>
+      </c>
+      <c r="H13" s="8">
+        <v>45912</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="7">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10670588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
+        <v>10738596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>10679792</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215BA176-A211-4AF1-BCC6-E15647AA23F6}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>

</xml_diff>